<commit_message>
modify testcases.xlsx kor to eng, but it needs review more
</commit_message>
<xml_diff>
--- a/MyDictionaryMVC/testcases.xlsx
+++ b/MyDictionaryMVC/testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\universe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MyDictionary\MyDictionaryMVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="301">
   <si>
     <t>SCOPE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>duplicated user add to user table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SELECT * FROM USER where userId = #{userId}
 then return User(testUser, name, testUser@gmail.com)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상응하는 유저 정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>search target user</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -223,14 +215,6 @@
     <t>isAlreadyFriendByIndex</t>
   </si>
   <si>
-    <t>user0과 user1이 친구 일 경우, 친구인지 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user0과 user1이 친구가 아닌 경우, 친구인지 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -239,29 +223,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>testUser0과 testUser1은 친구인가 == true</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>testUser2와 testUser1은 친구인가 == false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insertFriendByIndex</t>
   </si>
   <si>
-    <t>testData에서 정의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test data와 같음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중복 값 insert</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>catch duplicatedPrimarykeyException</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -308,63 +272,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>user의 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>찾음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>못찾음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정 성공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>delete target user from table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>친구 맞음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>친구 아님</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>친구 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>testUser0의 친구 리스트 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>testUser1의 친구 리스트 검색</t>
-  </si>
-  <si>
-    <t>testUser2의 친구 리스트 검색</t>
-  </si>
-  <si>
-    <t>testUser3의 친구 리스트 검색</t>
-  </si>
-  <si>
-    <t>testUser4의 친구 리스트 검색</t>
-  </si>
-  <si>
-    <t>user를 친구 추가한 다른 user의 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가한 사람이 없는 user를 친구 추가한 다른 user 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -568,10 +480,6 @@
   </si>
   <si>
     <t>result == null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상응하는 dictionary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -684,23 +592,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>count key에 대한 dictionary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>result == 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>count collection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>collection의 모든 element count</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User에 대한 Unit test는 google과 연동 되는 부분을 stub으로 정의하는 것이 너무 커서 스킵</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -789,10 +685,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상응하는 friend list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC_INT_USER_01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -881,18 +773,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>get dictionary 같은 keyword의 친구꺼 까지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>result == [{userId0__keyword, ...}, ..., {userId4__keyword, ...}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>친구의 dictionary 중 같은 keyword가 없는 경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>keyword = keyword + keyword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -909,14 +793,6 @@
   </si>
   <si>
     <t>findUserByEmail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user의 정보 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일치하는 user의 json type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -941,10 +817,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>user의 json type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>User(0, null, null, null, null)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1051,18 +923,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>testUser4의 친구 리스트 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>실패시 json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성공시 json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>testUser0's friends: testUser1, testUser2, testUser3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1149,7 +1009,168 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Document가 구현되면 해봐야뎀</t>
+    <t>found</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not found</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modify complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser0's friends list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser1's friends list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser2's friends list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser3's friends list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser4's friends list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not friends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user's list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defined in testData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the number of collection's all element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if failed, json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search user's information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if successed, json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser0's friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser1's friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser2's friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser3's friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search testUser4's friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user's json type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corresponding user information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>equals to test data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corresponding dictionary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>they are friends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert duplicated value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add user to user table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add duplicated user to user table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get other user's list that add user to friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">get other user's list that add user who has no friends to friend </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found user's json type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corresponding friend list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>** if Document part will be implemented, then test **</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get dictionaries about same keyword in friends' dictionaries</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>there is no documents about same keyword in friends' dictionaries</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If user0 and user1 are friends, check they are friends already.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If user0 and user1 are not friends, check they are friends already.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if testUser0 &amp;&amp; testUser1 are friends == true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if testUser2 &amp;&amp; testUser1 are friends == false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the number of dictionaries that has corresponding key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is too heavy to define a stub that is interlocked with google and user's unit test.
+So skipped.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1332,7 +1353,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1411,47 +1432,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1489,6 +1477,24 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1546,17 +1552,35 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="double">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1572,18 +1596,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="표2" displayName="표2" ref="B2:K82" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="표2" displayName="표2" ref="B2:K82" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="B2:K82"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="SCOPE" dataDxfId="8"/>
-    <tableColumn id="2" name="Test Case ID" dataDxfId="7"/>
+    <tableColumn id="1" name="SCOPE" dataDxfId="7"/>
+    <tableColumn id="2" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="3" name="Method Name"/>
-    <tableColumn id="4" name="Test Scenario" dataDxfId="6"/>
-    <tableColumn id="5" name="Expected Result" dataDxfId="5"/>
-    <tableColumn id="6" name="Test Data" dataDxfId="0"/>
-    <tableColumn id="7" name="Test Oracle" dataDxfId="4"/>
-    <tableColumn id="8" name="Actual Result" dataDxfId="3"/>
-    <tableColumn id="9" name="Result" dataDxfId="2"/>
+    <tableColumn id="4" name="Test Scenario" dataDxfId="5"/>
+    <tableColumn id="5" name="Expected Result" dataDxfId="4"/>
+    <tableColumn id="6" name="Test Data" dataDxfId="3"/>
+    <tableColumn id="7" name="Test Oracle" dataDxfId="2"/>
+    <tableColumn id="8" name="Actual Result" dataDxfId="1"/>
+    <tableColumn id="9" name="Result" dataDxfId="0"/>
     <tableColumn id="10" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1855,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1912,26 +1936,26 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>74</v>
+        <v>260</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -1940,26 +1964,26 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>261</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -1968,28 +1992,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>286</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -1998,28 +2022,28 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -2028,28 +2052,28 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>27</v>
+        <v>281</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>27</v>
+        <v>281</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -2058,26 +2082,26 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -2086,26 +2110,26 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>27</v>
+        <v>281</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>27</v>
+        <v>281</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -2114,26 +2138,26 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -2142,28 +2166,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -2172,28 +2196,28 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -2202,86 +2226,86 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>79</v>
+        <v>284</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -2290,28 +2314,28 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>58</v>
+        <v>282</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>58</v>
+        <v>282</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>58</v>
+        <v>282</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -2320,26 +2344,26 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -2348,28 +2372,28 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>263</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -2378,28 +2402,28 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>83</v>
+        <v>264</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -2408,28 +2432,28 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>265</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="2"/>
     </row>
@@ -2438,28 +2462,28 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="J21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K21" s="2"/>
     </row>
@@ -2468,28 +2492,28 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>86</v>
+        <v>267</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" s="2"/>
     </row>
@@ -2498,28 +2522,28 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>87</v>
+        <v>288</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>73</v>
+        <v>269</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2527,28 +2551,28 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
@@ -2556,28 +2580,28 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
@@ -2585,26 +2609,26 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
@@ -2619,28 +2643,28 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
@@ -2648,28 +2672,28 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>144</v>
+        <v>283</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
@@ -2677,28 +2701,28 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="81" x14ac:dyDescent="0.3">
@@ -2706,28 +2730,28 @@
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
@@ -2735,28 +2759,28 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="45" x14ac:dyDescent="0.3">
@@ -2764,28 +2788,28 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
@@ -2793,57 +2817,57 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>172</v>
+        <v>142</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
@@ -2851,28 +2875,28 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>175</v>
+        <v>271</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
@@ -2884,20 +2908,20 @@
       <c r="I37" s="3"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="E38" s="2"/>
       <c r="G38" s="7"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="2"/>
-      <c r="K38" t="s">
-        <v>176</v>
+      <c r="K38" s="26" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
@@ -2911,263 +2935,263 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="D40" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="D42" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="D46" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="D47" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D48" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>198</v>
+        <v>291</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
@@ -3181,147 +3205,147 @@
     </row>
     <row r="50" spans="2:10" ht="30" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>144</v>
+        <v>283</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="D51" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="30" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>224</v>
+        <v>195</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>293</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>144</v>
+        <v>283</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>226</v>
+        <v>195</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
@@ -3335,10 +3359,10 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="E56" s="2"/>
       <c r="G56" s="7"/>
@@ -3348,10 +3372,10 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="E57" s="2"/>
       <c r="G57" s="7"/>
@@ -3370,503 +3394,503 @@
     </row>
     <row r="59" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="D59" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>232</v>
+        <v>273</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>233</v>
+        <v>290</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="30" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
       <c r="D62" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>243</v>
+        <v>210</v>
       </c>
       <c r="D63" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
       <c r="D64" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="D65" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D67" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="D68" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>261</v>
+        <v>228</v>
       </c>
       <c r="D69" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="D70" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>264</v>
+        <v>231</v>
       </c>
       <c r="D71" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>82</v>
+        <v>275</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>83</v>
+        <v>276</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="D73" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>84</v>
+        <v>277</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="3"/>
@@ -3876,16 +3900,16 @@
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="D77" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="7"/>
@@ -3894,10 +3918,10 @@
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="3"/>
@@ -3907,10 +3931,10 @@
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="3"/>
@@ -3920,16 +3944,16 @@
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="D80" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="7"/>
@@ -3938,10 +3962,10 @@
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="3"/>
@@ -3951,10 +3975,10 @@
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="3"/>

</xml_diff>